<commit_message>
refactor: rename METHOD column to DERIVATION in Variables sheet
- Renamed METHOD → DERIVATION in Study_Metadata.xlsx Variables sheet
- Added empty METHOD column for backward reference
- Updated .read_variables_sheet() to read derivation column → internal method
  (with METHOD fallback for backward compatibility)
- Updated all comments, roxygen docs, vignettes, README, and docs/
- Regenerated .Rd files
- Pipeline tested: 115 rules compile and build_domain works correctly
</commit_message>
<xml_diff>
--- a/inst/extdata/starter_kit/metadata/Study_Metadata.xlsx
+++ b/inst/extdata/starter_kit/metadata/Study_Metadata.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="558">
   <si>
     <t xml:space="preserve">Select</t>
   </si>
@@ -1689,6 +1689,9 @@
   </si>
   <si>
     <t xml:space="preserve">HEIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DERIVATION</t>
   </si>
 </sst>
 </file>
@@ -3367,9 +3370,12 @@
         <v>60</v>
       </c>
       <c r="R1" t="s">
+        <v>557</v>
+      </c>
+      <c r="S1" t="s">
         <v>61</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3423,6 +3429,7 @@
         <v>68</v>
       </c>
       <c r="S2"/>
+      <c r="T2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -3474,6 +3481,7 @@
         <v>70</v>
       </c>
       <c r="S3"/>
+      <c r="T3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -3525,6 +3533,7 @@
         <v>73</v>
       </c>
       <c r="S4"/>
+      <c r="T4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -3576,6 +3585,7 @@
         <v>77</v>
       </c>
       <c r="S5"/>
+      <c r="T5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -3627,6 +3637,7 @@
         <v>82</v>
       </c>
       <c r="S6"/>
+      <c r="T6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -3678,6 +3689,7 @@
         <v>86</v>
       </c>
       <c r="S7"/>
+      <c r="T7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -3729,6 +3741,7 @@
         <v>91</v>
       </c>
       <c r="S8"/>
+      <c r="T8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -3780,6 +3793,7 @@
         <v>68</v>
       </c>
       <c r="S9"/>
+      <c r="T9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -3831,6 +3845,7 @@
         <v>92</v>
       </c>
       <c r="S10"/>
+      <c r="T10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -3882,6 +3897,7 @@
         <v>93</v>
       </c>
       <c r="S11"/>
+      <c r="T11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -3932,7 +3948,8 @@
       <c r="R12" t="s">
         <v>97</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S12"/>
+      <c r="T12" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3986,6 +4003,7 @@
         <v>103</v>
       </c>
       <c r="S13"/>
+      <c r="T13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -4037,6 +4055,7 @@
         <v>107</v>
       </c>
       <c r="S14"/>
+      <c r="T14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -4088,6 +4107,7 @@
         <v>111</v>
       </c>
       <c r="S15"/>
+      <c r="T15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -4136,7 +4156,8 @@
       <c r="R16" t="s">
         <v>117</v>
       </c>
-      <c r="S16" t="s">
+      <c r="S16"/>
+      <c r="T16" t="s">
         <v>118</v>
       </c>
     </row>
@@ -4190,6 +4211,7 @@
         <v>68</v>
       </c>
       <c r="S17"/>
+      <c r="T17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -4241,6 +4263,7 @@
         <v>119</v>
       </c>
       <c r="S18"/>
+      <c r="T18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -4292,6 +4315,7 @@
         <v>93</v>
       </c>
       <c r="S19"/>
+      <c r="T19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -4342,7 +4366,8 @@
       <c r="R20" t="s">
         <v>121</v>
       </c>
-      <c r="S20" t="s">
+      <c r="S20"/>
+      <c r="T20" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4398,6 +4423,7 @@
         <v>125</v>
       </c>
       <c r="S21"/>
+      <c r="T21"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -4451,6 +4477,7 @@
         <v>130</v>
       </c>
       <c r="S22"/>
+      <c r="T22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -4504,6 +4531,7 @@
         <v>136</v>
       </c>
       <c r="S23"/>
+      <c r="T23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -4557,6 +4585,7 @@
         <v>142</v>
       </c>
       <c r="S24"/>
+      <c r="T24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -4608,6 +4637,7 @@
         <v>68</v>
       </c>
       <c r="S25"/>
+      <c r="T25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -4659,6 +4689,7 @@
         <v>143</v>
       </c>
       <c r="S26"/>
+      <c r="T26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -4710,6 +4741,7 @@
         <v>93</v>
       </c>
       <c r="S27"/>
+      <c r="T27"/>
     </row>
     <row r="28">
       <c r="A28" t="s">
@@ -4760,7 +4792,8 @@
       <c r="R28" t="s">
         <v>121</v>
       </c>
-      <c r="S28" t="s">
+      <c r="S28"/>
+      <c r="T28" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4814,6 +4847,7 @@
         <v>148</v>
       </c>
       <c r="S29"/>
+      <c r="T29"/>
     </row>
     <row r="30">
       <c r="A30" t="s">
@@ -4865,6 +4899,7 @@
         <v>151</v>
       </c>
       <c r="S30"/>
+      <c r="T30"/>
     </row>
     <row r="31">
       <c r="A31" t="s">
@@ -4916,6 +4951,7 @@
         <v>154</v>
       </c>
       <c r="S31"/>
+      <c r="T31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -4965,6 +5001,7 @@
         <v>68</v>
       </c>
       <c r="S32"/>
+      <c r="T32"/>
     </row>
     <row r="33">
       <c r="A33" t="s">
@@ -5014,6 +5051,7 @@
         <v>216</v>
       </c>
       <c r="S33"/>
+      <c r="T33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
@@ -5063,6 +5101,7 @@
         <v>93</v>
       </c>
       <c r="S34"/>
+      <c r="T34"/>
     </row>
     <row r="35">
       <c r="A35" t="s">
@@ -5113,7 +5152,8 @@
       <c r="R35" t="s">
         <v>218</v>
       </c>
-      <c r="S35" t="s">
+      <c r="S35"/>
+      <c r="T35" t="s">
         <v>219</v>
       </c>
     </row>
@@ -5167,6 +5207,7 @@
         <v>222</v>
       </c>
       <c r="S36"/>
+      <c r="T36"/>
     </row>
     <row r="37">
       <c r="A37" t="s">
@@ -5218,6 +5259,7 @@
         <v>226</v>
       </c>
       <c r="S37"/>
+      <c r="T37"/>
     </row>
     <row r="38">
       <c r="A38" t="s">
@@ -5267,6 +5309,7 @@
         <v>229</v>
       </c>
       <c r="S38"/>
+      <c r="T38"/>
     </row>
     <row r="39">
       <c r="A39" t="s">
@@ -5318,6 +5361,7 @@
         <v>232</v>
       </c>
       <c r="S39"/>
+      <c r="T39"/>
     </row>
     <row r="40">
       <c r="A40" t="s">
@@ -5369,6 +5413,7 @@
         <v>235</v>
       </c>
       <c r="S40"/>
+      <c r="T40"/>
     </row>
     <row r="41">
       <c r="A41" t="s">
@@ -5420,6 +5465,7 @@
         <v>232</v>
       </c>
       <c r="S41"/>
+      <c r="T41"/>
     </row>
     <row r="42">
       <c r="A42" t="s">
@@ -5469,6 +5515,7 @@
         <v>240</v>
       </c>
       <c r="S42"/>
+      <c r="T42"/>
     </row>
     <row r="43">
       <c r="A43" t="s">
@@ -5518,6 +5565,7 @@
         <v>243</v>
       </c>
       <c r="S43"/>
+      <c r="T43"/>
     </row>
     <row r="44">
       <c r="A44" t="s">
@@ -5567,6 +5615,7 @@
         <v>246</v>
       </c>
       <c r="S44"/>
+      <c r="T44"/>
     </row>
     <row r="45">
       <c r="A45" t="s">
@@ -5617,7 +5666,8 @@
       <c r="R45" t="s">
         <v>251</v>
       </c>
-      <c r="S45" t="s">
+      <c r="S45"/>
+      <c r="T45" t="s">
         <v>252</v>
       </c>
     </row>
@@ -5663,6 +5713,7 @@
         <v>255</v>
       </c>
       <c r="S46"/>
+      <c r="T46"/>
     </row>
     <row r="47">
       <c r="A47" t="s">
@@ -5704,6 +5755,7 @@
         <v>538</v>
       </c>
       <c r="S47"/>
+      <c r="T47"/>
     </row>
     <row r="48">
       <c r="A48" t="s">
@@ -5745,6 +5797,7 @@
         <v>261</v>
       </c>
       <c r="S48"/>
+      <c r="T48"/>
     </row>
     <row r="49">
       <c r="A49" t="s">
@@ -5785,7 +5838,8 @@
       <c r="R49" t="s">
         <v>264</v>
       </c>
-      <c r="S49" t="s">
+      <c r="S49"/>
+      <c r="T49" t="s">
         <v>105</v>
       </c>
     </row>
@@ -5828,7 +5882,8 @@
       <c r="R50" t="s">
         <v>267</v>
       </c>
-      <c r="S50" t="s">
+      <c r="S50"/>
+      <c r="T50" t="s">
         <v>105</v>
       </c>
     </row>
@@ -5872,6 +5927,7 @@
         <v>270</v>
       </c>
       <c r="S51"/>
+      <c r="T51"/>
     </row>
     <row r="52">
       <c r="A52" t="s">
@@ -5913,6 +5969,7 @@
         <v>273</v>
       </c>
       <c r="S52"/>
+      <c r="T52"/>
     </row>
     <row r="53">
       <c r="A53" t="s">
@@ -5956,6 +6013,7 @@
         <v>276</v>
       </c>
       <c r="S53"/>
+      <c r="T53"/>
     </row>
     <row r="54">
       <c r="A54" t="s">
@@ -5997,6 +6055,7 @@
         <v>279</v>
       </c>
       <c r="S54"/>
+      <c r="T54"/>
     </row>
     <row r="55">
       <c r="A55" t="s">
@@ -6038,6 +6097,7 @@
         <v>282</v>
       </c>
       <c r="S55"/>
+      <c r="T55"/>
     </row>
     <row r="56">
       <c r="A56" t="s">
@@ -6079,6 +6139,7 @@
         <v>285</v>
       </c>
       <c r="S56"/>
+      <c r="T56"/>
     </row>
     <row r="57">
       <c r="A57" t="s">
@@ -6120,6 +6181,7 @@
         <v>288</v>
       </c>
       <c r="S57"/>
+      <c r="T57"/>
     </row>
     <row r="58">
       <c r="A58" t="s">
@@ -6163,6 +6225,7 @@
         <v>292</v>
       </c>
       <c r="S58"/>
+      <c r="T58"/>
     </row>
     <row r="59">
       <c r="A59" t="s">
@@ -6206,6 +6269,7 @@
         <v>296</v>
       </c>
       <c r="S59"/>
+      <c r="T59"/>
     </row>
     <row r="60">
       <c r="A60" t="s">
@@ -6248,7 +6312,8 @@
       <c r="R60" t="s">
         <v>299</v>
       </c>
-      <c r="S60" t="s">
+      <c r="S60"/>
+      <c r="T60" t="s">
         <v>132</v>
       </c>
     </row>
@@ -6292,6 +6357,7 @@
         <v>302</v>
       </c>
       <c r="S61"/>
+      <c r="T61"/>
     </row>
     <row r="62">
       <c r="A62" t="s">
@@ -6332,7 +6398,8 @@
       <c r="R62" t="s">
         <v>305</v>
       </c>
-      <c r="S62" t="s">
+      <c r="S62"/>
+      <c r="T62" t="s">
         <v>300</v>
       </c>
     </row>
@@ -6375,7 +6442,8 @@
       <c r="R63" t="s">
         <v>308</v>
       </c>
-      <c r="S63" t="s">
+      <c r="S63"/>
+      <c r="T63" t="s">
         <v>238</v>
       </c>
     </row>
@@ -6419,6 +6487,7 @@
         <v>311</v>
       </c>
       <c r="S64"/>
+      <c r="T64"/>
     </row>
     <row r="65">
       <c r="A65" t="s">
@@ -6459,7 +6528,8 @@
       <c r="R65" t="s">
         <v>314</v>
       </c>
-      <c r="S65" t="s">
+      <c r="S65"/>
+      <c r="T65" t="s">
         <v>227</v>
       </c>
     </row>
@@ -6502,7 +6572,8 @@
       <c r="R66" t="s">
         <v>317</v>
       </c>
-      <c r="S66" t="s">
+      <c r="S66"/>
+      <c r="T66" t="s">
         <v>318</v>
       </c>
     </row>
@@ -6546,6 +6617,7 @@
         <v>68</v>
       </c>
       <c r="S67"/>
+      <c r="T67"/>
     </row>
     <row r="68">
       <c r="A68" t="s">
@@ -6587,6 +6659,7 @@
         <v>320</v>
       </c>
       <c r="S68"/>
+      <c r="T68"/>
     </row>
     <row r="69">
       <c r="A69" t="s">
@@ -6628,6 +6701,7 @@
         <v>93</v>
       </c>
       <c r="S69"/>
+      <c r="T69"/>
     </row>
     <row r="70">
       <c r="A70" t="s">
@@ -6668,7 +6742,8 @@
       <c r="R70" t="s">
         <v>121</v>
       </c>
-      <c r="S70" t="s">
+      <c r="S70"/>
+      <c r="T70" t="s">
         <v>71</v>
       </c>
     </row>
@@ -6712,6 +6787,7 @@
         <v>324</v>
       </c>
       <c r="S71"/>
+      <c r="T71"/>
     </row>
     <row r="72">
       <c r="A72" t="s">
@@ -6755,6 +6831,7 @@
         <v>328</v>
       </c>
       <c r="S72"/>
+      <c r="T72"/>
     </row>
     <row r="73">
       <c r="A73" t="s">
@@ -6798,6 +6875,7 @@
         <v>331</v>
       </c>
       <c r="S73"/>
+      <c r="T73"/>
     </row>
     <row r="74">
       <c r="A74" t="s">
@@ -6839,6 +6917,7 @@
         <v>334</v>
       </c>
       <c r="S74"/>
+      <c r="T74"/>
     </row>
     <row r="75">
       <c r="A75" t="s">
@@ -6880,6 +6959,7 @@
         <v>68</v>
       </c>
       <c r="S75"/>
+      <c r="T75"/>
     </row>
     <row r="76">
       <c r="A76" t="s">
@@ -6921,6 +7001,7 @@
         <v>336</v>
       </c>
       <c r="S76"/>
+      <c r="T76"/>
     </row>
     <row r="77">
       <c r="A77" t="s">
@@ -6962,6 +7043,7 @@
         <v>93</v>
       </c>
       <c r="S77"/>
+      <c r="T77"/>
     </row>
     <row r="78">
       <c r="A78" t="s">
@@ -7002,7 +7084,8 @@
       <c r="R78" t="s">
         <v>121</v>
       </c>
-      <c r="S78" t="s">
+      <c r="S78"/>
+      <c r="T78" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7046,6 +7129,7 @@
         <v>340</v>
       </c>
       <c r="S79"/>
+      <c r="T79"/>
     </row>
     <row r="80">
       <c r="A80" t="s">
@@ -7087,6 +7171,7 @@
         <v>343</v>
       </c>
       <c r="S80"/>
+      <c r="T80"/>
     </row>
     <row r="81">
       <c r="A81" t="s">
@@ -7130,6 +7215,7 @@
         <v>346</v>
       </c>
       <c r="S81"/>
+      <c r="T81"/>
     </row>
     <row r="82">
       <c r="A82" t="s">
@@ -7173,6 +7259,7 @@
         <v>348</v>
       </c>
       <c r="S82"/>
+      <c r="T82"/>
     </row>
     <row r="83">
       <c r="A83" t="s">
@@ -7216,6 +7303,7 @@
         <v>350</v>
       </c>
       <c r="S83"/>
+      <c r="T83"/>
     </row>
     <row r="84">
       <c r="A84" t="s">
@@ -7257,6 +7345,7 @@
         <v>353</v>
       </c>
       <c r="S84"/>
+      <c r="T84"/>
     </row>
     <row r="85">
       <c r="A85" t="s">
@@ -7298,6 +7387,7 @@
         <v>356</v>
       </c>
       <c r="S85"/>
+      <c r="T85"/>
     </row>
     <row r="86">
       <c r="A86" t="s">
@@ -7339,6 +7429,7 @@
         <v>68</v>
       </c>
       <c r="S86"/>
+      <c r="T86"/>
     </row>
     <row r="87">
       <c r="A87" t="s">
@@ -7380,6 +7471,7 @@
         <v>358</v>
       </c>
       <c r="S87"/>
+      <c r="T87"/>
     </row>
     <row r="88">
       <c r="A88" t="s">
@@ -7421,6 +7513,7 @@
         <v>93</v>
       </c>
       <c r="S88"/>
+      <c r="T88"/>
     </row>
     <row r="89">
       <c r="A89" t="s">
@@ -7461,7 +7554,8 @@
       <c r="R89" t="s">
         <v>121</v>
       </c>
-      <c r="S89" t="s">
+      <c r="S89"/>
+      <c r="T89" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7505,6 +7599,7 @@
         <v>362</v>
       </c>
       <c r="S90"/>
+      <c r="T90"/>
     </row>
     <row r="91">
       <c r="A91" t="s">
@@ -7546,6 +7641,7 @@
         <v>364</v>
       </c>
       <c r="S91"/>
+      <c r="T91"/>
     </row>
     <row r="92">
       <c r="A92" t="s">
@@ -7587,6 +7683,7 @@
         <v>367</v>
       </c>
       <c r="S92"/>
+      <c r="T92"/>
     </row>
     <row r="93">
       <c r="A93" t="s">
@@ -7628,6 +7725,7 @@
         <v>370</v>
       </c>
       <c r="S93"/>
+      <c r="T93"/>
     </row>
     <row r="94">
       <c r="A94" t="s">
@@ -7669,6 +7767,7 @@
         <v>373</v>
       </c>
       <c r="S94"/>
+      <c r="T94"/>
     </row>
     <row r="95">
       <c r="A95" t="s">
@@ -7710,6 +7809,7 @@
         <v>68</v>
       </c>
       <c r="S95"/>
+      <c r="T95"/>
     </row>
     <row r="96">
       <c r="A96" t="s">
@@ -7751,6 +7851,7 @@
         <v>375</v>
       </c>
       <c r="S96"/>
+      <c r="T96"/>
     </row>
     <row r="97">
       <c r="A97" t="s">
@@ -7792,6 +7893,7 @@
         <v>93</v>
       </c>
       <c r="S97"/>
+      <c r="T97"/>
     </row>
     <row r="98">
       <c r="A98" t="s">
@@ -7832,7 +7934,8 @@
       <c r="R98" t="s">
         <v>121</v>
       </c>
-      <c r="S98" t="s">
+      <c r="S98"/>
+      <c r="T98" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7876,6 +7979,7 @@
         <v>379</v>
       </c>
       <c r="S99"/>
+      <c r="T99"/>
     </row>
     <row r="100">
       <c r="A100" t="s">
@@ -7917,6 +8021,7 @@
         <v>382</v>
       </c>
       <c r="S100"/>
+      <c r="T100"/>
     </row>
     <row r="101">
       <c r="A101" t="s">
@@ -7958,6 +8063,7 @@
         <v>385</v>
       </c>
       <c r="S101"/>
+      <c r="T101"/>
     </row>
     <row r="102">
       <c r="A102" t="s">
@@ -7999,6 +8105,7 @@
         <v>388</v>
       </c>
       <c r="S102"/>
+      <c r="T102"/>
     </row>
     <row r="103">
       <c r="A103" t="s">
@@ -8040,6 +8147,7 @@
         <v>390</v>
       </c>
       <c r="S103"/>
+      <c r="T103"/>
     </row>
     <row r="104">
       <c r="A104" t="s">
@@ -8081,6 +8189,7 @@
         <v>393</v>
       </c>
       <c r="S104"/>
+      <c r="T104"/>
     </row>
     <row r="105">
       <c r="A105" t="s">
@@ -8122,6 +8231,7 @@
         <v>539</v>
       </c>
       <c r="S105"/>
+      <c r="T105"/>
     </row>
     <row r="106">
       <c r="A106" t="s">
@@ -8163,6 +8273,7 @@
         <v>399</v>
       </c>
       <c r="S106"/>
+      <c r="T106"/>
     </row>
     <row r="107">
       <c r="A107" t="s">
@@ -8204,6 +8315,7 @@
         <v>525</v>
       </c>
       <c r="S107"/>
+      <c r="T107"/>
     </row>
     <row r="108">
       <c r="A108" t="s">
@@ -8245,6 +8357,7 @@
         <v>513</v>
       </c>
       <c r="S108"/>
+      <c r="T108"/>
     </row>
     <row r="109">
       <c r="A109" t="s">
@@ -8286,6 +8399,7 @@
         <v>246</v>
       </c>
       <c r="S109"/>
+      <c r="T109"/>
     </row>
     <row r="110">
       <c r="A110" t="s">
@@ -8326,7 +8440,8 @@
       <c r="R110" t="s">
         <v>528</v>
       </c>
-      <c r="S110" t="s">
+      <c r="S110"/>
+      <c r="T110" t="s">
         <v>391</v>
       </c>
     </row>
@@ -8370,6 +8485,7 @@
         <v>243</v>
       </c>
       <c r="S111"/>
+      <c r="T111"/>
     </row>
     <row r="112">
       <c r="A112" t="s">
@@ -8411,6 +8527,7 @@
         <v>529</v>
       </c>
       <c r="S112"/>
+      <c r="T112"/>
     </row>
     <row r="113">
       <c r="A113" t="s">
@@ -8453,7 +8570,8 @@
       <c r="R113" t="s">
         <v>532</v>
       </c>
-      <c r="S113" t="s">
+      <c r="S113"/>
+      <c r="T113" t="s">
         <v>123</v>
       </c>
     </row>
@@ -8497,6 +8615,7 @@
         <v>514</v>
       </c>
       <c r="S114"/>
+      <c r="T114"/>
     </row>
     <row r="115">
       <c r="A115" t="s">
@@ -8538,6 +8657,7 @@
         <v>518</v>
       </c>
       <c r="S115"/>
+      <c r="T115"/>
     </row>
     <row r="116">
       <c r="A116" t="s">
@@ -8579,6 +8699,7 @@
         <v>517</v>
       </c>
       <c r="S116"/>
+      <c r="T116"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>